<commit_message>
fix xml data model error
</commit_message>
<xml_diff>
--- a/mime/application%vnd.openxmlformats-officedocument.spreadsheetml.sheet/test/themed.xlsx
+++ b/mime/application%vnd.openxmlformats-officedocument.spreadsheetml.sheet/test/themed.xlsx
@@ -16,9 +16,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>AAAAAAA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AAAAS</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -26,7 +30,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -52,6 +56,13 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="26"/>
+      <color theme="4"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -67,7 +78,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -75,13 +86,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -411,123 +438,237 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="5" max="5" width="20.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A1">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:14" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:14" ht="37.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A7">
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="E7" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="F12">
+        <v>6</v>
+      </c>
+      <c r="G12">
+        <v>7</v>
+      </c>
+      <c r="H12">
+        <v>8</v>
+      </c>
+      <c r="I12">
+        <v>9</v>
+      </c>
+      <c r="J12">
+        <v>10</v>
+      </c>
+      <c r="K12">
+        <v>11</v>
+      </c>
+      <c r="L12">
+        <v>12</v>
+      </c>
+      <c r="M12">
+        <v>13</v>
+      </c>
+      <c r="N12">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>7</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C14">
+        <v>7</v>
+      </c>
+      <c r="D14">
+        <v>10</v>
+      </c>
+      <c r="E14">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C15">
+        <v>9</v>
+      </c>
+      <c r="D15">
+        <v>13</v>
+      </c>
+      <c r="E15">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="C16">
+        <v>11</v>
+      </c>
+      <c r="D16">
+        <v>16</v>
+      </c>
+      <c r="E16">
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="C17">
+        <v>13</v>
+      </c>
+      <c r="D17">
+        <v>19</v>
+      </c>
+      <c r="E17">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="C18">
+        <v>15</v>
+      </c>
+      <c r="D18">
+        <v>22</v>
+      </c>
+      <c r="E18">
+        <v>-13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="C19">
+        <v>17</v>
+      </c>
+      <c r="D19">
+        <v>25</v>
+      </c>
+      <c r="E19">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="C20">
+        <v>19</v>
+      </c>
+      <c r="D20">
+        <v>28</v>
+      </c>
+      <c r="E20">
+        <v>-19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>22</v>
       </c>
@@ -535,7 +676,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -543,6 +684,28 @@
         <color rgb="FF5A8AC6"/>
         <color rgb="FFFCFCFF"/>
         <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12:E20">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F12:N12">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEF9C"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>

</xml_diff>